<commit_message>
simulating closing positions added
</commit_message>
<xml_diff>
--- a/etc/Events.xlsx
+++ b/etc/Events.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -48,18 +48,12 @@
     <t>DepositAccounted</t>
   </si>
   <si>
-    <t>SavingsPlanRateAccounted</t>
-  </si>
-  <si>
     <t>Event</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>some text</t>
-  </si>
-  <si>
     <t>GB001100110</t>
   </si>
   <si>
@@ -88,6 +82,15 @@
   </si>
   <si>
     <t>Paul AG</t>
+  </si>
+  <si>
+    <t>savings plan</t>
+  </si>
+  <si>
+    <t>special loan received</t>
+  </si>
+  <si>
+    <t>PositionClosed</t>
   </si>
 </sst>
 </file>
@@ -445,11 +448,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,16 +470,16 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -488,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -499,10 +502,10 @@
         <v>41640</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -514,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -525,10 +528,10 @@
         <v>41731</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -548,10 +551,10 @@
         <v>41773</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="7">
@@ -569,10 +572,10 @@
         <v>41791</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5">
         <v>5</v>
@@ -592,10 +595,10 @@
         <v>41792</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="5">
         <v>200</v>
@@ -615,10 +618,10 @@
         <v>41821</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="6">
         <v>100</v>
@@ -638,10 +641,10 @@
         <v>41831</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7">
@@ -664,12 +667,12 @@
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>41913</v>
@@ -681,6 +684,9 @@
         <v>500</v>
       </c>
       <c r="G10" s="7"/>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -690,10 +696,10 @@
         <v>42083</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5">
         <v>15</v>
@@ -713,10 +719,10 @@
         <v>42166</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7">
@@ -762,10 +768,10 @@
         <v>42495</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
@@ -785,10 +791,10 @@
         <v>42532</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7">
@@ -804,10 +810,10 @@
         <v>42653</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" s="5">
         <v>10</v>
@@ -816,6 +822,24 @@
         <v>150</v>
       </c>
       <c r="G17" s="7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="8">
+        <v>4</v>
+      </c>
+      <c r="G18" s="7">
         <v>9.9</v>
       </c>
     </row>

</xml_diff>